<commit_message>
Small additions to test documentation (half done)
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUFF\Documents\Egyetem\szakdolgozat\szakdolgozat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E45517F-F739-4C76-A589-838577DA7316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3D3FB-8DF1-4E7D-A2A1-4D90BF2AEE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16B1F42F-497A-4036-8175-4FEE2FD02B2C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{16B1F42F-497A-4036-8175-4FEE2FD02B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -208,6 +208,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -540,9 +546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B00C75-DBA2-4DD4-8C14-92195DEE5212}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q62" sqref="Q62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3323,7 +3329,7 @@
         <v>10</v>
       </c>
       <c r="E62" s="13">
-        <f t="shared" si="1"/>
+        <f>D62/B62</f>
         <v>1</v>
       </c>
       <c r="F62" s="8">
@@ -3438,45 +3444,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
+    <row r="65" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="16">
         <v>64</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="17">
         <v>15</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="17">
         <v>15</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="17">
         <v>15</v>
       </c>
-      <c r="E65" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F65" s="8">
-        <v>2</v>
-      </c>
-      <c r="G65" s="12">
+      <c r="E65" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F65" s="17">
+        <v>2</v>
+      </c>
+      <c r="G65" s="19">
         <v>12</v>
       </c>
-      <c r="H65" s="12">
+      <c r="H65" s="19">
         <v>-1</v>
       </c>
-      <c r="S65" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="T65" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U65" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V65" s="2">
+      <c r="S65" s="16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T65" s="16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U65" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V65" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3518,13 +3524,26 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
-      <c r="F67">
+      <c r="C67" s="14">
+        <f>C66/B66</f>
+        <v>0.99459459459459465</v>
+      </c>
+      <c r="D67" s="14">
+        <f>D66/C66</f>
+        <v>0.98913043478260865</v>
+      </c>
+      <c r="F67" s="15">
         <f>SUM(F2:F65)/F66</f>
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
+      <c r="D68" s="14">
+        <f>D66/B66</f>
+        <v>0.98378378378378384</v>
+      </c>
+      <c r="F68" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M21">

</xml_diff>

<commit_message>
Tests, canvas small fix
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUFF\Documents\Egyetem\szakdolgozat\szakdolgozat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3D3FB-8DF1-4E7D-A2A1-4D90BF2AEE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E79F8D-147D-4EBC-BA89-B3A5E6E54413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{16B1F42F-497A-4036-8175-4FEE2FD02B2C}"/>
   </bookViews>
@@ -544,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B00C75-DBA2-4DD4-8C14-92195DEE5212}">
-  <dimension ref="A1:V68"/>
+  <dimension ref="A1:V77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3536,6 +3536,13 @@
         <f>SUM(F2:F65)/F66</f>
         <v>2</v>
       </c>
+      <c r="H67">
+        <v>-5</v>
+      </c>
+      <c r="I67">
+        <f>COUNTIFS($H$2:$H$65,H67)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
@@ -3544,6 +3551,94 @@
         <v>0.98378378378378384</v>
       </c>
       <c r="F68" s="15"/>
+      <c r="H68">
+        <v>-4</v>
+      </c>
+      <c r="I68">
+        <f t="shared" ref="I68:I78" si="4">COUNTIFS($H$2:$H$65,H68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H69">
+        <v>-3</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H70">
+        <v>-2</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H71">
+        <v>-1</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H75">
+        <v>3</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H76">
+        <v>4</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H77">
+        <v>5</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M21">

</xml_diff>